<commit_message>
0.0.13 - Change Upload System
</commit_message>
<xml_diff>
--- a/Source/Excel/Loads_01.xlsx
+++ b/Source/Excel/Loads_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>*</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>-5</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>value2</t>
   </si>
 </sst>
 </file>
@@ -506,7 +518,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,16 +562,16 @@
         <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
0.0.14 - Add Nodal and Member Concentrated Load
</commit_message>
<xml_diff>
--- a/Source/Excel/Loads_01.xlsx
+++ b/Source/Excel/Loads_01.xlsx
@@ -59,9 +59,6 @@
     <t>direction</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>FX</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>value2</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,19 +559,19 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -596,11 +596,11 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="1">
         <v>5</v>
       </c>
@@ -611,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -622,10 +622,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -648,10 +648,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -663,7 +663,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -683,13 +683,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1">
         <v>5</v>
@@ -713,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -721,13 +721,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -739,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -751,16 +751,8 @@
         <v>5</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="I9" s="11"/>
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>